<commit_message>
Updated the paradigm sheets
</commit_message>
<xml_diff>
--- a/Paradigm Practice Sheets.xlsx
+++ b/Paradigm Practice Sheets.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lmurphey/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lmurphey/git/learning_biblical_hebrew_flashcards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC87E0A-1DB7-EB48-B513-B81615E98810}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757F2FCC-BEF4-CD47-B6A5-FEA2EB14F7F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{4C87BD8E-1E8C-C245-855C-B75398CF1004}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="37640" windowHeight="21140" activeTab="3" xr2:uid="{4C87BD8E-1E8C-C245-855C-B75398CF1004}"/>
   </bookViews>
   <sheets>
     <sheet name="Verb" sheetId="1" r:id="rId1"/>
     <sheet name="Noun" sheetId="3" r:id="rId2"/>
+    <sheet name="Verb (perfect imperfect)" sheetId="4" r:id="rId3"/>
+    <sheet name="Noun (forms)" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,19 +36,73 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="20">
   <si>
     <t>שׁמר</t>
   </si>
   <si>
     <t>סוּס</t>
   </si>
+  <si>
+    <t>Imperfect</t>
+  </si>
+  <si>
+    <t>Perfect</t>
+  </si>
+  <si>
+    <t>Masc</t>
+  </si>
+  <si>
+    <t>Fem</t>
+  </si>
+  <si>
+    <t>Plural</t>
+  </si>
+  <si>
+    <t>שָׁמַר</t>
+  </si>
+  <si>
+    <t>שָֽׁמְרָה</t>
+  </si>
+  <si>
+    <t>שָֽׁמְרוּ</t>
+  </si>
+  <si>
+    <t>יִשְׁמֹר</t>
+  </si>
+  <si>
+    <t>תִּשְׁמֹר</t>
+  </si>
+  <si>
+    <t>יִשְׁמְרוּ</t>
+  </si>
+  <si>
+    <t>Singular</t>
+  </si>
+  <si>
+    <t>Dual</t>
+  </si>
+  <si>
+    <t>סוּסִים</t>
+  </si>
+  <si>
+    <t>סוּסַ֫יִם</t>
+  </si>
+  <si>
+    <t>סוּסָה</t>
+  </si>
+  <si>
+    <t>סוּסוֹת</t>
+  </si>
+  <si>
+    <t>סוּסָתַ֫יִם</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -68,6 +124,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -77,7 +156,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -85,14 +164,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="2"/>
     </xf>
   </cellXfs>
@@ -411,7 +567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{447A2566-54B9-A94D-89CF-EA16990C57A9}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1212,7 +1368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8506E0-DCB5-E548-8147-9106134BEDE6}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -1803,4 +1959,1448 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2376BC-DBFD-154D-A23B-AF47B3CE2A9A}">
+  <dimension ref="A1:G38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="31" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="12" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" style="1" customWidth="1"/>
+    <col min="5" max="7" width="12" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+    </row>
+    <row r="2" spans="1:7" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+    </row>
+    <row r="21" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="E20:G20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F4E82F-20A4-114F-B9A0-20D04133CB11}">
+  <dimension ref="A1:F39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="31" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="14.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="1" customWidth="1"/>
+    <col min="5" max="6" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+    </row>
+    <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A20" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+    </row>
+    <row r="21" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:F20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding more practice sheets
</commit_message>
<xml_diff>
--- a/Paradigm Practice Sheets.xlsx
+++ b/Paradigm Practice Sheets.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lmurphey/git/learning_biblical_hebrew_flashcards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76327CB-F53E-5B4C-B893-452FC9B28BA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6693A21D-746D-C843-A860-543A5A137443}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="32840" windowHeight="20540" activeTab="4" xr2:uid="{4C87BD8E-1E8C-C245-855C-B75398CF1004}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="33600" windowHeight="21000" activeTab="6" xr2:uid="{4C87BD8E-1E8C-C245-855C-B75398CF1004}"/>
   </bookViews>
   <sheets>
     <sheet name="Verb" sheetId="1" r:id="rId1"/>
     <sheet name="Noun" sheetId="3" r:id="rId2"/>
     <sheet name="Verb (perfect imperfect)" sheetId="4" r:id="rId3"/>
     <sheet name="Noun (forms)" sheetId="6" r:id="rId4"/>
-    <sheet name="That, this" sheetId="7" r:id="rId5"/>
+    <sheet name="Contruct Forms" sheetId="9" r:id="rId5"/>
+    <sheet name="That, this" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="45">
   <si>
     <t>שׁמר</t>
   </si>
@@ -139,6 +141,39 @@
   </si>
   <si>
     <t>הֵן ,הֵ֫נָּה</t>
+  </si>
+  <si>
+    <t>סוּס-֫</t>
+  </si>
+  <si>
+    <t>סוּסֵי-֫</t>
+  </si>
+  <si>
+    <t>סוּסוֹת-֫</t>
+  </si>
+  <si>
+    <t>סוּסַת-֫</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Long</t>
   </si>
 </sst>
 </file>
@@ -380,7 +415,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -416,22 +451,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -454,6 +474,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2180,17 +2223,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
       <c r="D1" s="8"/>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:7" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -2555,17 +2598,17 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
     </row>
     <row r="21" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
@@ -2944,7 +2987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F4E82F-20A4-114F-B9A0-20D04133CB11}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -2957,16 +3000,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="45"/>
       <c r="C1" s="12"/>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
     </row>
     <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -3277,16 +3320,16 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="24"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="12"/>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
     </row>
     <row r="21" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
@@ -3609,11 +3652,570 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF5A6BC-C11A-0E45-9DEE-DEAF7BFB8F64}">
+  <dimension ref="A1:E39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="31" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="14.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="47"/>
+    </row>
+    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A20" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="45"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="47"/>
+    </row>
+    <row r="21" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:E20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15438D8A-5D82-4B49-BC3F-E9F4A1820D7A}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3631,384 +4233,384 @@
       <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="23" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="30" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="30"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="42"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="30"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="42"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="30"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="25"/>
     </row>
     <row r="6" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="42"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="30"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="42"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="30"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="42"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="30"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="25"/>
     </row>
     <row r="9" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="42"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="30"/>
+      <c r="A9" s="37"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="25"/>
     </row>
     <row r="10" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="42"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="30"/>
+      <c r="A10" s="37"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="25"/>
     </row>
     <row r="11" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="42"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="30"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="25"/>
     </row>
     <row r="12" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="42"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="30"/>
+      <c r="A12" s="37"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="25"/>
     </row>
     <row r="13" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="42"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="30"/>
+      <c r="A13" s="37"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="25"/>
     </row>
     <row r="14" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="42"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="30"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="25"/>
     </row>
     <row r="15" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="42"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="30"/>
+      <c r="A15" s="37"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="25"/>
     </row>
     <row r="16" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="42"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="30"/>
+      <c r="A16" s="37"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="25"/>
     </row>
     <row r="17" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="42"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="30"/>
+      <c r="A17" s="37"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="25"/>
     </row>
     <row r="18" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="42"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="30"/>
+      <c r="A18" s="37"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="25"/>
     </row>
     <row r="19" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="44"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="27"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="22"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="46" t="s">
+      <c r="D20" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="29" t="s">
+      <c r="E20" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="29" t="s">
+      <c r="F20" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="29" t="s">
+      <c r="G20" s="24" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="32" t="s">
+      <c r="D21" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="34" t="s">
+      <c r="F21" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="G21" s="35" t="s">
+      <c r="G21" s="30" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="42"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="30"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="25"/>
     </row>
     <row r="23" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="42"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="30"/>
+      <c r="A23" s="37"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="25"/>
     </row>
     <row r="24" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="42"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="30"/>
+      <c r="A24" s="37"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="25"/>
     </row>
     <row r="25" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="42"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="30"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="25"/>
     </row>
     <row r="26" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="42"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="30"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="25"/>
     </row>
     <row r="27" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="42"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="30"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="25"/>
     </row>
     <row r="28" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="42"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="30"/>
+      <c r="A28" s="37"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="25"/>
     </row>
     <row r="29" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="42"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="30"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="25"/>
     </row>
     <row r="30" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="42"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="30"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="25"/>
     </row>
     <row r="31" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="42"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="30"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="25"/>
     </row>
     <row r="32" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="42"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="30"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="25"/>
     </row>
     <row r="33" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="42"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="30"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="25"/>
     </row>
     <row r="34" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="42"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="30"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="25"/>
     </row>
     <row r="35" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="42"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="30"/>
+      <c r="A35" s="37"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="25"/>
     </row>
     <row r="36" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="42"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="30"/>
+      <c r="A36" s="37"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="25"/>
     </row>
     <row r="37" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="42"/>
-      <c r="B37" s="37"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="30"/>
+      <c r="A37" s="37"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="25"/>
     </row>
     <row r="38" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4018,4 +4620,803 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9187CC4-7C5D-724F-A0F9-D4348E82F7CE}">
+  <dimension ref="A1:J66"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="10" width="8.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+    </row>
+    <row r="2" spans="1:10" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+    </row>
+    <row r="4" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+    </row>
+    <row r="5" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+    </row>
+    <row r="6" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+    </row>
+    <row r="7" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+    </row>
+    <row r="8" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+    </row>
+    <row r="9" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+    </row>
+    <row r="10" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+    </row>
+    <row r="11" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+    </row>
+    <row r="12" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+    </row>
+    <row r="13" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+    </row>
+    <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+    </row>
+    <row r="15" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+    </row>
+    <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+    </row>
+    <row r="17" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+    </row>
+    <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+    </row>
+    <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+    </row>
+    <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+    </row>
+    <row r="21" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+    </row>
+    <row r="22" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+    </row>
+    <row r="23" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+    </row>
+    <row r="24" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="32"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+    </row>
+    <row r="25" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="32"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+    </row>
+    <row r="26" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="32"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+    </row>
+    <row r="27" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+    </row>
+    <row r="28" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+    </row>
+    <row r="29" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+    </row>
+    <row r="30" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="32"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+    </row>
+    <row r="31" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="G31" s="44"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="44"/>
+    </row>
+    <row r="32" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="H32" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="I32" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="J32" s="48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="32"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+    </row>
+    <row r="34" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="32"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
+      <c r="J34" s="32"/>
+    </row>
+    <row r="35" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="32"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
+      <c r="J35" s="32"/>
+    </row>
+    <row r="36" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="32"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+    </row>
+    <row r="37" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="32"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="32"/>
+    </row>
+    <row r="38" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="32"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="32"/>
+      <c r="J38" s="32"/>
+    </row>
+    <row r="39" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="32"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="32"/>
+    </row>
+    <row r="40" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="32"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="32"/>
+    </row>
+    <row r="41" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="32"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="32"/>
+      <c r="J41" s="32"/>
+    </row>
+    <row r="42" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="32"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="32"/>
+    </row>
+    <row r="43" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="32"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="32"/>
+    </row>
+    <row r="44" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="32"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32"/>
+      <c r="J44" s="32"/>
+    </row>
+    <row r="45" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="32"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
+    </row>
+    <row r="46" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="32"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="32"/>
+    </row>
+    <row r="47" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="32"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="32"/>
+      <c r="J47" s="32"/>
+    </row>
+    <row r="48" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="32"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="32"/>
+      <c r="I48" s="32"/>
+      <c r="J48" s="32"/>
+    </row>
+    <row r="49" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="32"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="32"/>
+      <c r="J49" s="32"/>
+    </row>
+    <row r="50" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="32"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="32"/>
+      <c r="J50" s="32"/>
+    </row>
+    <row r="51" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="32"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="32"/>
+      <c r="J51" s="32"/>
+    </row>
+    <row r="52" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="32"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="32"/>
+      <c r="J52" s="32"/>
+    </row>
+    <row r="53" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="32"/>
+      <c r="B53" s="32"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="32"/>
+      <c r="F53" s="32"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="32"/>
+      <c r="I53" s="32"/>
+      <c r="J53" s="32"/>
+    </row>
+    <row r="54" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="32"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="32"/>
+      <c r="H54" s="32"/>
+      <c r="I54" s="32"/>
+      <c r="J54" s="32"/>
+    </row>
+    <row r="55" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="32"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="32"/>
+      <c r="F55" s="32"/>
+      <c r="G55" s="32"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="32"/>
+      <c r="J55" s="32"/>
+    </row>
+    <row r="56" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="32"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="32"/>
+      <c r="I56" s="32"/>
+      <c r="J56" s="32"/>
+    </row>
+    <row r="57" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="32"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="32"/>
+      <c r="F57" s="32"/>
+      <c r="G57" s="32"/>
+      <c r="H57" s="32"/>
+      <c r="I57" s="32"/>
+      <c r="J57" s="32"/>
+    </row>
+    <row r="58" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="32"/>
+      <c r="B58" s="32"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="32"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="32"/>
+      <c r="G58" s="32"/>
+      <c r="H58" s="32"/>
+      <c r="I58" s="32"/>
+      <c r="J58" s="32"/>
+    </row>
+    <row r="59" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="32"/>
+      <c r="B59" s="32"/>
+      <c r="C59" s="32"/>
+      <c r="D59" s="32"/>
+      <c r="E59" s="32"/>
+      <c r="F59" s="32"/>
+      <c r="G59" s="32"/>
+      <c r="H59" s="32"/>
+      <c r="I59" s="32"/>
+      <c r="J59" s="32"/>
+    </row>
+    <row r="60" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="32"/>
+      <c r="B60" s="32"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="32"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="32"/>
+      <c r="G60" s="32"/>
+      <c r="H60" s="32"/>
+      <c r="I60" s="32"/>
+      <c r="J60" s="32"/>
+    </row>
+    <row r="61" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="F31:J31"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating the numbers sheets
</commit_message>
<xml_diff>
--- a/Paradigm Practice Sheets.xlsx
+++ b/Paradigm Practice Sheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lmurphey/git/learning_biblical_hebrew_flashcards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3876DA47-C835-4E4C-9A42-C84A85435EBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B9735D-91FB-104E-A19D-9686F4AB9248}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="460" windowWidth="37640" windowHeight="21140" activeTab="8" xr2:uid="{4C87BD8E-1E8C-C245-855C-B75398CF1004}"/>
   </bookViews>
@@ -445,7 +445,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -626,11 +626,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -697,6 +741,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -718,8 +763,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2446,17 +2505,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
       <c r="D1" s="8"/>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
     </row>
     <row r="2" spans="1:7" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -2821,17 +2880,17 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="49" t="s">
+      <c r="E20" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="50"/>
-      <c r="G20" s="50"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
     </row>
     <row r="21" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
@@ -3223,16 +3282,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="51"/>
+      <c r="B1" s="52"/>
       <c r="C1" s="12"/>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
     </row>
     <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -3543,16 +3602,16 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="51" t="s">
+      <c r="A20" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="51"/>
+      <c r="B20" s="52"/>
       <c r="C20" s="12"/>
-      <c r="D20" s="52" t="s">
+      <c r="D20" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
     </row>
     <row r="21" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
@@ -3891,15 +3950,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="51"/>
+      <c r="B1" s="52"/>
       <c r="C1" s="21"/>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="53"/>
+      <c r="E1" s="54"/>
     </row>
     <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -4156,15 +4215,15 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="51" t="s">
+      <c r="A20" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="51"/>
+      <c r="B20" s="52"/>
       <c r="C20" s="21"/>
-      <c r="D20" s="52" t="s">
+      <c r="D20" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="53"/>
+      <c r="E20" s="54"/>
     </row>
     <row r="21" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
@@ -4859,20 +4918,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="49" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
@@ -5243,20 +5302,20 @@
       <c r="J30" s="32"/>
     </row>
     <row r="31" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="48" t="s">
+      <c r="A31" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="48"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="49" t="s">
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="50"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
     </row>
     <row r="32" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="42" t="s">
@@ -6238,328 +6297,426 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X22" sqref="X22"/>
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="31" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="10.83203125" style="3"/>
+    <col min="5" max="5" width="11.33203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="13" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13" style="55" customWidth="1"/>
+    <col min="7" max="7" width="13" style="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="42" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="55"/>
+      <c r="G1" s="48"/>
     </row>
     <row r="2" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="61" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="58" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="58" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="58" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="58" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="58" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="58" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="58" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="57" t="s">
         <v>93</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="58" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="58" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="A12" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="57" t="s">
         <v>95</v>
       </c>
+      <c r="F12" s="62"/>
     </row>
     <row r="13" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="57" t="s">
         <v>96</v>
       </c>
+      <c r="F13" s="63"/>
     </row>
     <row r="14" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="57" t="s">
         <v>97</v>
       </c>
+      <c r="F14" s="63"/>
     </row>
     <row r="15" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="A15" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="57" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="56"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="42" t="s">
+      <c r="F15" s="63"/>
+    </row>
+    <row r="16" spans="1:7" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="64"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="F16" s="42" t="s">
+      <c r="F16" s="65" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="61" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="A18" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="58" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="58" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="A20" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="58" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="A21" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="58" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="A22" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="58" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="A23" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="58" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="A24" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="58" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="A25" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="57" t="s">
         <v>93</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="58" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="A26" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="58" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="A27" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="57" t="s">
         <v>95</v>
       </c>
+      <c r="F27" s="62"/>
     </row>
     <row r="28" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="A28" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="57" t="s">
         <v>96</v>
       </c>
+      <c r="F28" s="63"/>
     </row>
     <row r="29" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="A29" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="57" t="s">
         <v>97</v>
       </c>
+      <c r="F29" s="63"/>
     </row>
     <row r="30" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="A30" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="57" t="s">
         <v>98</v>
       </c>
+      <c r="F30" s="63"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A16:D16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <rowBreaks count="1" manualBreakCount="1">

</xml_diff>

<commit_message>
New paradigms for qal
</commit_message>
<xml_diff>
--- a/Paradigm Practice Sheets.xlsx
+++ b/Paradigm Practice Sheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lmurphey/git/learning_biblical_hebrew_flashcards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B9735D-91FB-104E-A19D-9686F4AB9248}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BD4A23-EFAE-1742-BAF0-AF334C2054F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="37640" windowHeight="21140" activeTab="8" xr2:uid="{4C87BD8E-1E8C-C245-855C-B75398CF1004}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="9" xr2:uid="{4C87BD8E-1E8C-C245-855C-B75398CF1004}"/>
   </bookViews>
   <sheets>
     <sheet name="Verb" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Vowels" sheetId="10" r:id="rId7"/>
     <sheet name="Pronominal" sheetId="14" r:id="rId8"/>
     <sheet name="Numbers" sheetId="15" r:id="rId9"/>
+    <sheet name="Qal" sheetId="16" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="120">
   <si>
     <t>שׁמר</t>
   </si>
@@ -362,13 +363,52 @@
   </si>
   <si>
     <t>עֲשִׂירִי</t>
+  </si>
+  <si>
+    <t>Qal Perfect Singular</t>
+  </si>
+  <si>
+    <t>Qal Perfect Plural</t>
+  </si>
+  <si>
+    <t>קטל</t>
+  </si>
+  <si>
+    <t>קָטַל</t>
+  </si>
+  <si>
+    <t xml:space="preserve">קָֽטְלָה </t>
+  </si>
+  <si>
+    <t xml:space="preserve">קָטַ֫לְתָּ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">קָטַלְתְּ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">קָטַ֫לְתִּי </t>
+  </si>
+  <si>
+    <t xml:space="preserve">קָֽטְלוּ </t>
+  </si>
+  <si>
+    <t>קְטַלְתֶּם</t>
+  </si>
+  <si>
+    <t xml:space="preserve">קְטַלְתֶּן </t>
+  </si>
+  <si>
+    <t xml:space="preserve">קָטַ֫לְנוּ </t>
+  </si>
+  <si>
+    <t>3cp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -436,6 +476,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -445,7 +491,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -670,11 +716,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -742,6 +799,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -763,12 +827,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -778,7 +836,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1892,6 +1951,549 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29973FD7-6173-1B40-91F3-9C61A2BF5DFD}">
+  <dimension ref="A1:E39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:E34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="31" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="5" width="14.5" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+    </row>
+    <row r="2" spans="1:5" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="66" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="67" t="s">
+        <v>113</v>
+      </c>
+      <c r="E17" s="67" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+    </row>
+    <row r="19" spans="1:5" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="46" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" s="67"/>
+      <c r="C34" s="67" t="s">
+        <v>116</v>
+      </c>
+      <c r="D34" s="67" t="s">
+        <v>117</v>
+      </c>
+      <c r="E34" s="67" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="17" max="16383" man="1"/>
+  </rowBreaks>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8506E0-DCB5-E548-8147-9106134BEDE6}">
   <dimension ref="A1:E34"/>
@@ -2505,17 +3107,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
       <c r="D1" s="8"/>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
     </row>
     <row r="2" spans="1:7" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -2880,17 +3482,17 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="49" t="s">
+      <c r="A20" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="50" t="s">
+      <c r="E20" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="51"/>
-      <c r="G20" s="51"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
     </row>
     <row r="21" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
@@ -3282,16 +3884,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="59"/>
       <c r="C1" s="12"/>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
     </row>
     <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -3602,16 +4204,16 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="52" t="s">
+      <c r="A20" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="52"/>
+      <c r="B20" s="59"/>
       <c r="C20" s="12"/>
-      <c r="D20" s="53" t="s">
+      <c r="D20" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
     </row>
     <row r="21" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
@@ -3950,15 +4552,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="59"/>
       <c r="C1" s="21"/>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="54"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -4215,15 +4817,15 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="52" t="s">
+      <c r="A20" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="52"/>
+      <c r="B20" s="59"/>
       <c r="C20" s="21"/>
-      <c r="D20" s="53" t="s">
+      <c r="D20" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="54"/>
+      <c r="E20" s="61"/>
     </row>
     <row r="21" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
@@ -4918,20 +5520,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="50" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
@@ -5302,20 +5904,20 @@
       <c r="J30" s="32"/>
     </row>
     <row r="31" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="49"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="50" t="s">
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="58"/>
+      <c r="J31" s="58"/>
     </row>
     <row r="32" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="42" t="s">
@@ -5708,7 +6310,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="X31" sqref="X31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="31" x14ac:dyDescent="0.35"/>
@@ -6296,7 +6898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4529F1D7-7DB7-604A-9ACC-50003AD2A9C1}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
@@ -6310,29 +6912,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="64"/>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65" t="s">
+      <c r="A1" s="65"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="65" t="s">
+      <c r="F1" s="55" t="s">
         <v>85</v>
       </c>
       <c r="G1" s="48"/>
     </row>
     <row r="2" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="60" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="61" t="s">
+      <c r="F2" s="54" t="s">
         <v>67</v>
       </c>
     </row>
@@ -6343,10 +6945,10 @@
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
-      <c r="E3" s="57" t="s">
+      <c r="E3" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="F3" s="58" t="s">
+      <c r="F3" s="51" t="s">
         <v>82</v>
       </c>
     </row>
@@ -6357,10 +6959,10 @@
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="F4" s="58" t="s">
+      <c r="F4" s="51" t="s">
         <v>99</v>
       </c>
     </row>
@@ -6371,10 +6973,10 @@
       <c r="B5" s="28"/>
       <c r="C5" s="28"/>
       <c r="D5" s="28"/>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="F5" s="58" t="s">
+      <c r="F5" s="51" t="s">
         <v>100</v>
       </c>
     </row>
@@ -6385,10 +6987,10 @@
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
       <c r="D6" s="28"/>
-      <c r="E6" s="57" t="s">
+      <c r="E6" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="F6" s="58" t="s">
+      <c r="F6" s="51" t="s">
         <v>101</v>
       </c>
     </row>
@@ -6399,10 +7001,10 @@
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
-      <c r="E7" s="57" t="s">
+      <c r="E7" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="58" t="s">
+      <c r="F7" s="51" t="s">
         <v>102</v>
       </c>
     </row>
@@ -6413,10 +7015,10 @@
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
-      <c r="E8" s="57" t="s">
+      <c r="E8" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="F8" s="58" t="s">
+      <c r="F8" s="51" t="s">
         <v>103</v>
       </c>
     </row>
@@ -6427,10 +7029,10 @@
       <c r="B9" s="28"/>
       <c r="C9" s="28"/>
       <c r="D9" s="28"/>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="F9" s="58" t="s">
+      <c r="F9" s="51" t="s">
         <v>104</v>
       </c>
     </row>
@@ -6441,10 +7043,10 @@
       <c r="B10" s="28"/>
       <c r="C10" s="28"/>
       <c r="D10" s="28"/>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="F10" s="58" t="s">
+      <c r="F10" s="51" t="s">
         <v>105</v>
       </c>
     </row>
@@ -6455,10 +7057,10 @@
       <c r="B11" s="28"/>
       <c r="C11" s="28"/>
       <c r="D11" s="28"/>
-      <c r="E11" s="57" t="s">
+      <c r="E11" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="F11" s="58" t="s">
+      <c r="F11" s="51" t="s">
         <v>106</v>
       </c>
     </row>
@@ -6469,10 +7071,10 @@
       <c r="B12" s="28"/>
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
-      <c r="E12" s="57" t="s">
+      <c r="E12" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="F12" s="62"/>
+      <c r="F12" s="63"/>
     </row>
     <row r="13" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="37" t="s">
@@ -6481,10 +7083,10 @@
       <c r="B13" s="28"/>
       <c r="C13" s="28"/>
       <c r="D13" s="28"/>
-      <c r="E13" s="57" t="s">
+      <c r="E13" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="F13" s="63"/>
+      <c r="F13" s="64"/>
     </row>
     <row r="14" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="37" t="s">
@@ -6493,10 +7095,10 @@
       <c r="B14" s="28"/>
       <c r="C14" s="28"/>
       <c r="D14" s="28"/>
-      <c r="E14" s="57" t="s">
+      <c r="E14" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="F14" s="63"/>
+      <c r="F14" s="64"/>
     </row>
     <row r="15" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="37" t="s">
@@ -6505,34 +7107,34 @@
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
-      <c r="E15" s="57" t="s">
+      <c r="E15" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="F15" s="63"/>
+      <c r="F15" s="64"/>
     </row>
     <row r="16" spans="1:7" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="64"/>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="65" t="s">
+      <c r="A16" s="65"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="F16" s="65" t="s">
+      <c r="F16" s="55" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="60" t="s">
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="F17" s="61" t="s">
+      <c r="F17" s="54" t="s">
         <v>67</v>
       </c>
     </row>
@@ -6543,10 +7145,10 @@
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
-      <c r="E18" s="57" t="s">
+      <c r="E18" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="58" t="s">
+      <c r="F18" s="51" t="s">
         <v>82</v>
       </c>
     </row>
@@ -6557,10 +7159,10 @@
       <c r="B19" s="28"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
-      <c r="E19" s="57" t="s">
+      <c r="E19" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="F19" s="58" t="s">
+      <c r="F19" s="51" t="s">
         <v>99</v>
       </c>
     </row>
@@ -6571,10 +7173,10 @@
       <c r="B20" s="28"/>
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>
-      <c r="E20" s="57" t="s">
+      <c r="E20" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="F20" s="58" t="s">
+      <c r="F20" s="51" t="s">
         <v>100</v>
       </c>
     </row>
@@ -6585,10 +7187,10 @@
       <c r="B21" s="28"/>
       <c r="C21" s="28"/>
       <c r="D21" s="28"/>
-      <c r="E21" s="57" t="s">
+      <c r="E21" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="F21" s="58" t="s">
+      <c r="F21" s="51" t="s">
         <v>101</v>
       </c>
     </row>
@@ -6599,10 +7201,10 @@
       <c r="B22" s="28"/>
       <c r="C22" s="28"/>
       <c r="D22" s="28"/>
-      <c r="E22" s="57" t="s">
+      <c r="E22" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="58" t="s">
+      <c r="F22" s="51" t="s">
         <v>102</v>
       </c>
     </row>
@@ -6613,10 +7215,10 @@
       <c r="B23" s="28"/>
       <c r="C23" s="28"/>
       <c r="D23" s="28"/>
-      <c r="E23" s="57" t="s">
+      <c r="E23" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="F23" s="58" t="s">
+      <c r="F23" s="51" t="s">
         <v>103</v>
       </c>
     </row>
@@ -6627,10 +7229,10 @@
       <c r="B24" s="28"/>
       <c r="C24" s="28"/>
       <c r="D24" s="28"/>
-      <c r="E24" s="57" t="s">
+      <c r="E24" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="F24" s="58" t="s">
+      <c r="F24" s="51" t="s">
         <v>104</v>
       </c>
     </row>
@@ -6641,10 +7243,10 @@
       <c r="B25" s="28"/>
       <c r="C25" s="28"/>
       <c r="D25" s="28"/>
-      <c r="E25" s="57" t="s">
+      <c r="E25" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="F25" s="58" t="s">
+      <c r="F25" s="51" t="s">
         <v>105</v>
       </c>
     </row>
@@ -6655,10 +7257,10 @@
       <c r="B26" s="28"/>
       <c r="C26" s="28"/>
       <c r="D26" s="28"/>
-      <c r="E26" s="57" t="s">
+      <c r="E26" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="F26" s="58" t="s">
+      <c r="F26" s="51" t="s">
         <v>106</v>
       </c>
     </row>
@@ -6669,10 +7271,10 @@
       <c r="B27" s="28"/>
       <c r="C27" s="28"/>
       <c r="D27" s="28"/>
-      <c r="E27" s="57" t="s">
+      <c r="E27" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="F27" s="62"/>
+      <c r="F27" s="63"/>
     </row>
     <row r="28" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="37" t="s">
@@ -6681,10 +7283,10 @@
       <c r="B28" s="28"/>
       <c r="C28" s="28"/>
       <c r="D28" s="28"/>
-      <c r="E28" s="57" t="s">
+      <c r="E28" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="F28" s="63"/>
+      <c r="F28" s="64"/>
     </row>
     <row r="29" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="37" t="s">
@@ -6693,10 +7295,10 @@
       <c r="B29" s="28"/>
       <c r="C29" s="28"/>
       <c r="D29" s="28"/>
-      <c r="E29" s="57" t="s">
+      <c r="E29" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="F29" s="63"/>
+      <c r="F29" s="64"/>
     </row>
     <row r="30" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="37" t="s">
@@ -6705,10 +7307,10 @@
       <c r="B30" s="28"/>
       <c r="C30" s="28"/>
       <c r="D30" s="28"/>
-      <c r="E30" s="57" t="s">
+      <c r="E30" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="F30" s="63"/>
+      <c r="F30" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Adding participles and infinitives
</commit_message>
<xml_diff>
--- a/Paradigm Practice Sheets.xlsx
+++ b/Paradigm Practice Sheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lmurphey/git/learning_biblical_hebrew_flashcards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBF4BAE-87ED-A640-BB34-9EB557A13906}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4F795E-1888-A44B-9F78-4371F77CF2F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="32840" windowHeight="20540" activeTab="10" xr2:uid="{4C87BD8E-1E8C-C245-855C-B75398CF1004}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="32840" windowHeight="20540" activeTab="11" xr2:uid="{4C87BD8E-1E8C-C245-855C-B75398CF1004}"/>
   </bookViews>
   <sheets>
     <sheet name="Verb" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Numbers" sheetId="15" r:id="rId9"/>
     <sheet name="Qal Perfect" sheetId="16" r:id="rId10"/>
     <sheet name="Qal Imperfect" sheetId="17" r:id="rId11"/>
+    <sheet name="Qal Participles" sheetId="18" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1562" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="144">
   <si>
     <t>שׁמר</t>
   </si>
@@ -433,6 +434,48 @@
   </si>
   <si>
     <t>נִקְטֹל</t>
+  </si>
+  <si>
+    <t>Qal Passive Participle</t>
+  </si>
+  <si>
+    <t>Qal Active Participle</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>mp</t>
+  </si>
+  <si>
+    <t>fs</t>
+  </si>
+  <si>
+    <t>fp</t>
+  </si>
+  <si>
+    <t>קֹטֵל</t>
+  </si>
+  <si>
+    <t>קֹטְלָה</t>
+  </si>
+  <si>
+    <t>קֹטְלִים</t>
+  </si>
+  <si>
+    <t>קֹטְלוֹת</t>
+  </si>
+  <si>
+    <t>קָטוּל</t>
+  </si>
+  <si>
+    <t>קְטוּלָה</t>
+  </si>
+  <si>
+    <t>קְטוּלִים</t>
+  </si>
+  <si>
+    <t>קְטוּלוֹת</t>
   </si>
 </sst>
 </file>
@@ -2529,7 +2572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4122085C-B827-3F46-B8E0-AA8F6FEB86D3}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A17" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A17" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
@@ -3105,6 +3148,497 @@
     <row r="37" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="38" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="39" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="17" max="16383" man="1"/>
+  </rowBreaks>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BBF04C3-304E-5D43-B04A-3FF0AB83EF66}">
+  <dimension ref="A1:D39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="31" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="4" width="19.5" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+    </row>
+    <row r="2" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="57" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" s="56" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="D17" s="57" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+    </row>
+    <row r="19" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" s="46" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="57" t="s">
+        <v>140</v>
+      </c>
+      <c r="B34" s="57" t="s">
+        <v>142</v>
+      </c>
+      <c r="C34" s="57" t="s">
+        <v>141</v>
+      </c>
+      <c r="D34" s="57" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding chapter 19 paradigms
</commit_message>
<xml_diff>
--- a/Paradigm Practice Sheets.xlsx
+++ b/Paradigm Practice Sheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lmurphey/git/learning_biblical_hebrew_flashcards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A027521E-8088-EC42-948B-3D1EEEEC16D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B04C0D-D5C3-E54F-AA33-6DA083A8DC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3860" yWindow="860" windowWidth="32840" windowHeight="20540" activeTab="12" xr2:uid="{4C87BD8E-1E8C-C245-855C-B75398CF1004}"/>
+    <workbookView xWindow="38400" yWindow="10580" windowWidth="33600" windowHeight="20500" activeTab="13" xr2:uid="{4C87BD8E-1E8C-C245-855C-B75398CF1004}"/>
   </bookViews>
   <sheets>
     <sheet name="Verb" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,13 @@
     <sheet name="Contruct Forms" sheetId="9" r:id="rId5"/>
     <sheet name="That, this" sheetId="7" r:id="rId6"/>
     <sheet name="Vowels" sheetId="10" r:id="rId7"/>
-    <sheet name="Pronominal" sheetId="14" r:id="rId8"/>
-    <sheet name="Numbers" sheetId="15" r:id="rId9"/>
-    <sheet name="Qal Perfect" sheetId="16" r:id="rId10"/>
-    <sheet name="Qal Imperfect" sheetId="17" r:id="rId11"/>
-    <sheet name="Qal Participles" sheetId="18" r:id="rId12"/>
-    <sheet name="Sheet1" sheetId="19" r:id="rId13"/>
+    <sheet name="Main Forms" sheetId="19" r:id="rId8"/>
+    <sheet name="Pronominal" sheetId="14" r:id="rId9"/>
+    <sheet name="Numbers" sheetId="15" r:id="rId10"/>
+    <sheet name="Qal Perfect" sheetId="16" r:id="rId11"/>
+    <sheet name="Qal Imperfect" sheetId="17" r:id="rId12"/>
+    <sheet name="Qal Participles" sheetId="18" r:id="rId13"/>
+    <sheet name="Piel, Pual, Hithpael" sheetId="21" r:id="rId14"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1884" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2082" uniqueCount="164">
   <si>
     <t>שׁמר</t>
   </si>
@@ -501,6 +502,42 @@
   </si>
   <si>
     <t>קָטוֹל</t>
+  </si>
+  <si>
+    <t>Piel</t>
+  </si>
+  <si>
+    <t>Pual</t>
+  </si>
+  <si>
+    <t>Hithpael</t>
+  </si>
+  <si>
+    <t>קַטֵּל</t>
+  </si>
+  <si>
+    <t>מְקַטֵּל</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> קִטֵּל</t>
+  </si>
+  <si>
+    <t>Ptc.</t>
+  </si>
+  <si>
+    <t>קֻטַּל</t>
+  </si>
+  <si>
+    <t>קֻטֹּל</t>
+  </si>
+  <si>
+    <t>מְקֻטָּל</t>
+  </si>
+  <si>
+    <t>הִתְקַטֵּל</t>
+  </si>
+  <si>
+    <t>מִתְקַטֵּל</t>
   </si>
 </sst>
 </file>
@@ -1001,6 +1038,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1031,22 +1084,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2161,10 +2198,443 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4529F1D7-7DB7-604A-9ACC-50003AD2A9C1}">
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA3" sqref="AA3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="31" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="11.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13" style="48" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="81"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="48"/>
+    </row>
+    <row r="2" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="54" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="51" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="51" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="51" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="51" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="51" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="51" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" s="51" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="79"/>
+    </row>
+    <row r="13" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="80"/>
+    </row>
+    <row r="14" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" s="80"/>
+    </row>
+    <row r="15" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" s="80"/>
+    </row>
+    <row r="16" spans="1:7" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="81"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="55" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="54" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" s="51" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="51" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="51" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="51" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" s="51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" s="51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="51" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="51" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" s="51" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="79"/>
+    </row>
+    <row r="28" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" s="80"/>
+    </row>
+    <row r="29" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" s="80"/>
+    </row>
+    <row r="30" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" s="80"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A16:D16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="15" max="16383" man="1"/>
+  </rowBreaks>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29973FD7-6173-1B40-91F3-9C61A2BF5DFD}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A14" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -2703,7 +3173,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4122085C-B827-3F46-B8E0-AA8F6FEB86D3}">
   <dimension ref="A1:E39"/>
   <sheetViews>
@@ -3292,12 +3762,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BBF04C3-304E-5D43-B04A-3FF0AB83EF66}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A18" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A15" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="31" x14ac:dyDescent="0.35"/>
@@ -3783,75 +4253,54 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63C65C7-1D87-E543-A04B-84291704A758}">
-  <dimension ref="A1:H24"/>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F552AE25-CC3E-D247-9704-FB16A32357CF}">
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H24"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="31" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="11.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="1" customWidth="1"/>
+    <col min="2" max="7" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="75" t="s">
+    <row r="1" spans="1:8" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="44" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="65" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="C1" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="E1" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="G1" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="H1" s="77" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="71" t="s">
-        <v>147</v>
-      </c>
-      <c r="B2" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E2" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="F2" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="G2" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="H2" s="69" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="71" t="s">
+      <c r="B2" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="67" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="61" t="s">
         <v>144</v>
       </c>
       <c r="B3" s="57" t="s">
@@ -3872,12 +4321,12 @@
       <c r="G3" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="68" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="71" t="s">
+      <c r="H3" s="58" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="61" t="s">
         <v>149</v>
       </c>
       <c r="B4" s="57" t="s">
@@ -3898,13 +4347,13 @@
       <c r="G4" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="H4" s="68" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="71" t="s">
-        <v>146</v>
+      <c r="H4" s="58" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="61" t="s">
+        <v>158</v>
       </c>
       <c r="B5" s="57" t="s">
         <v>109</v>
@@ -3924,65 +4373,44 @@
       <c r="G5" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="H5" s="68" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="72" t="s">
-        <v>145</v>
-      </c>
-      <c r="B6" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="C6" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="E6" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="F6" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="G6" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="H6" s="74" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="75" t="s">
+      <c r="H5" s="58" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="44" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="65" t="s">
         <v>148</v>
       </c>
-      <c r="B7" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="C7" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="E7" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="F7" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="G7" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="H7" s="77" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="71" t="s">
-        <v>147</v>
+      <c r="B7" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="H7" s="67" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="61" t="s">
+        <v>144</v>
       </c>
       <c r="B8" s="57" t="s">
         <v>109</v>
@@ -4002,404 +4430,341 @@
       <c r="G8" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="H8" s="69" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="71" t="s">
+      <c r="H8" s="59" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="61" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G9" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" s="58" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="61" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F10" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G10" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H10" s="58" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="44" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="65" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="H12" s="67" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="61" t="s">
         <v>144</v>
       </c>
-      <c r="B9" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="C9" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="D9" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E9" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="F9" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="G9" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="H9" s="68" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="71" t="s">
+      <c r="B13" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G13" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H13" s="59" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="61" t="s">
         <v>149</v>
       </c>
-      <c r="B10" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="C10" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="D10" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E10" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="F10" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="G10" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="H10" s="68" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="71" t="s">
-        <v>146</v>
-      </c>
-      <c r="B11" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="C11" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="D11" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E11" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="F11" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="G11" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="H11" s="68" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="81" t="s">
-        <v>145</v>
-      </c>
-      <c r="B12" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="C12" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="D12" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="E12" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="F12" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="G12" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="H12" s="74" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="75" t="s">
+      <c r="B14" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" s="58" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="61" t="s">
+        <v>158</v>
+      </c>
+      <c r="B15" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E15" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G15" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" s="58" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="44" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="65" t="s">
         <v>148</v>
       </c>
-      <c r="B13" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="E13" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="F13" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="G13" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="H13" s="77" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="71" t="s">
-        <v>147</v>
-      </c>
-      <c r="B14" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="D14" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E14" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="F14" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="G14" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="H14" s="69" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="71" t="s">
+      <c r="B17" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="H17" s="67" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="61" t="s">
         <v>144</v>
       </c>
-      <c r="B15" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="C15" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="D15" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E15" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="F15" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="G15" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="H15" s="68" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="71" t="s">
+      <c r="B18" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" s="58" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="61" t="s">
         <v>149</v>
       </c>
-      <c r="B16" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="C16" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="D16" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E16" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="F16" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="G16" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="H16" s="68" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="71" t="s">
-        <v>146</v>
-      </c>
-      <c r="B17" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="D17" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E17" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="F17" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="G17" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="H17" s="68" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="72" t="s">
-        <v>145</v>
-      </c>
-      <c r="B18" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="C18" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="D18" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="E18" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="F18" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="G18" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="H18" s="74" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="78" t="s">
+      <c r="B19" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H19" s="58" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="61" t="s">
+        <v>158</v>
+      </c>
+      <c r="B20" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G20" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H20" s="58" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="44" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="65" t="s">
         <v>148</v>
       </c>
-      <c r="B19" s="79" t="s">
-        <v>109</v>
-      </c>
-      <c r="C19" s="79" t="s">
-        <v>109</v>
-      </c>
-      <c r="D19" s="79" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" s="79" t="s">
-        <v>109</v>
-      </c>
-      <c r="F19" s="79" t="s">
-        <v>109</v>
-      </c>
-      <c r="G19" s="79" t="s">
-        <v>109</v>
-      </c>
-      <c r="H19" s="80" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="71" t="s">
-        <v>147</v>
-      </c>
-      <c r="B20" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="C20" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="D20" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E20" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="F20" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="G20" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="H20" s="69" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="71" t="s">
+      <c r="B22" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="G22" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22" s="67" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="61" t="s">
         <v>144</v>
       </c>
-      <c r="B21" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="C21" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="D21" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E21" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="F21" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="G21" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="H21" s="68" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="71" t="s">
+      <c r="B23" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E23" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H23" s="59" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="61" t="s">
         <v>149</v>
       </c>
-      <c r="B22" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="C22" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="D22" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="F22" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="G22" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="H22" s="68" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="71" t="s">
-        <v>146</v>
-      </c>
-      <c r="B23" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="C23" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="D23" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E23" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="F23" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="G23" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="H23" s="68" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="70" t="s">
-        <v>145</v>
-      </c>
       <c r="B24" s="57" t="s">
         <v>109</v>
       </c>
@@ -4418,15 +4783,150 @@
       <c r="G24" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="H24" s="68" t="s">
-        <v>140</v>
+      <c r="H24" s="58" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="61" t="s">
+        <v>158</v>
+      </c>
+      <c r="B25" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G25" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H25" s="58" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="44" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="65" t="s">
+        <v>148</v>
+      </c>
+      <c r="B27" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="G27" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="H27" s="67" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="61" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F28" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G28" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H28" s="59" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="61" t="s">
+        <v>149</v>
+      </c>
+      <c r="B29" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F29" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G29" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H29" s="58" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="61" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E30" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G30" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H30" s="58" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="86" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="12" max="16383" man="1"/>
+    <brk id="15" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
@@ -5044,17 +5544,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
       <c r="D1" s="8"/>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
     </row>
     <row r="2" spans="1:7" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -5419,17 +5919,17 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="58"/>
-      <c r="C20" s="58"/>
+      <c r="B20" s="72"/>
+      <c r="C20" s="72"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="59" t="s">
+      <c r="E20" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="60"/>
-      <c r="G20" s="60"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="74"/>
     </row>
     <row r="21" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
@@ -5821,16 +6321,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="61"/>
+      <c r="B1" s="75"/>
       <c r="C1" s="12"/>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
     </row>
     <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -6141,16 +6641,16 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="61"/>
+      <c r="B20" s="75"/>
       <c r="C20" s="12"/>
-      <c r="D20" s="62" t="s">
+      <c r="D20" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="77"/>
     </row>
     <row r="21" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
@@ -6489,15 +6989,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="61"/>
+      <c r="B1" s="75"/>
       <c r="C1" s="21"/>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="63"/>
+      <c r="E1" s="77"/>
     </row>
     <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -6754,15 +7254,15 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="61"/>
+      <c r="B20" s="75"/>
       <c r="C20" s="21"/>
-      <c r="D20" s="62" t="s">
+      <c r="D20" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="63"/>
+      <c r="E20" s="77"/>
     </row>
     <row r="21" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
@@ -7457,20 +7957,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="59" t="s">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
@@ -7841,20 +8341,20 @@
       <c r="J30" s="32"/>
     </row>
     <row r="31" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="58" t="s">
+      <c r="A31" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="58"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="59" t="s">
+      <c r="B31" s="72"/>
+      <c r="C31" s="72"/>
+      <c r="D31" s="72"/>
+      <c r="E31" s="78"/>
+      <c r="F31" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="G31" s="60"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="60"/>
-      <c r="J31" s="60"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="74"/>
+      <c r="I31" s="74"/>
+      <c r="J31" s="74"/>
     </row>
     <row r="32" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="42" t="s">
@@ -8243,6 +8743,654 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63C65C7-1D87-E543-A04B-84291704A758}">
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="31" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="11.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="65" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="H1" s="67" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="61" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="59" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="61" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="58" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="61" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" s="58" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="61" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" s="58" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="62" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="H6" s="64" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="65" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="H7" s="67" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="61" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H8" s="59" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="61" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G9" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" s="58" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="61" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F10" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G10" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H10" s="58" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="61" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G11" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="58" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="71" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="H12" s="64" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="65" t="s">
+        <v>148</v>
+      </c>
+      <c r="B13" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="G13" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="H13" s="67" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="61" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" s="59" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="61" t="s">
+        <v>144</v>
+      </c>
+      <c r="B15" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E15" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G15" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" s="58" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="61" t="s">
+        <v>149</v>
+      </c>
+      <c r="B16" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G16" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" s="58" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="61" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H17" s="58" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="62" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" s="64" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="68" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19" s="69" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="69" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="69" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" s="69" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" s="69" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" s="69" t="s">
+        <v>109</v>
+      </c>
+      <c r="H19" s="70" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="61" t="s">
+        <v>147</v>
+      </c>
+      <c r="B20" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G20" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H20" s="59" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="61" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G21" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" s="58" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="61" t="s">
+        <v>149</v>
+      </c>
+      <c r="B22" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G22" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22" s="58" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="61" t="s">
+        <v>146</v>
+      </c>
+      <c r="B23" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E23" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H23" s="58" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="60" t="s">
+        <v>145</v>
+      </c>
+      <c r="B24" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G24" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H24" s="58" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="12" max="16383" man="1"/>
+  </rowBreaks>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200FC52B-DE55-42A9-8472-ED6B8297B8BA}">
   <dimension ref="A1:E39"/>
   <sheetViews>
@@ -8829,437 +9977,4 @@
     <brk id="17" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4529F1D7-7DB7-604A-9ACC-50003AD2A9C1}">
-  <dimension ref="A1:G30"/>
-  <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="31" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="11.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13" style="48" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="67"/>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="55" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="G1" s="48"/>
-    </row>
-    <row r="2" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="53" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" s="54" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="50" t="s">
-        <v>86</v>
-      </c>
-      <c r="F3" s="51" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="50" t="s">
-        <v>87</v>
-      </c>
-      <c r="F4" s="51" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="50" t="s">
-        <v>88</v>
-      </c>
-      <c r="F5" s="51" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="50" t="s">
-        <v>89</v>
-      </c>
-      <c r="F6" s="51" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="50" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7" s="51" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="50" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" s="51" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="F9" s="51" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="50" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" s="51" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="F11" s="51" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="50" t="s">
-        <v>95</v>
-      </c>
-      <c r="F12" s="65"/>
-    </row>
-    <row r="13" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="F13" s="66"/>
-    </row>
-    <row r="14" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="50" t="s">
-        <v>97</v>
-      </c>
-      <c r="F14" s="66"/>
-    </row>
-    <row r="15" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="50" t="s">
-        <v>98</v>
-      </c>
-      <c r="F15" s="66"/>
-    </row>
-    <row r="16" spans="1:7" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="67"/>
-      <c r="B16" s="67"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="55" t="s">
-        <v>84</v>
-      </c>
-      <c r="F16" s="55" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="53" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="54" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="50" t="s">
-        <v>86</v>
-      </c>
-      <c r="F18" s="51" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="50" t="s">
-        <v>87</v>
-      </c>
-      <c r="F19" s="51" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="50" t="s">
-        <v>88</v>
-      </c>
-      <c r="F20" s="51" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="50" t="s">
-        <v>89</v>
-      </c>
-      <c r="F21" s="51" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="50" t="s">
-        <v>90</v>
-      </c>
-      <c r="F22" s="51" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="50" t="s">
-        <v>91</v>
-      </c>
-      <c r="F23" s="51" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="F24" s="51" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="50" t="s">
-        <v>93</v>
-      </c>
-      <c r="F25" s="51" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="F26" s="51" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="50" t="s">
-        <v>95</v>
-      </c>
-      <c r="F27" s="65"/>
-    </row>
-    <row r="28" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="F28" s="66"/>
-    </row>
-    <row r="29" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="50" t="s">
-        <v>97</v>
-      </c>
-      <c r="F29" s="66"/>
-    </row>
-    <row r="30" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="50" t="s">
-        <v>98</v>
-      </c>
-      <c r="F30" s="66"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A16:D16"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="15" max="16383" man="1"/>
-  </rowBreaks>
-</worksheet>
 </file>
</xml_diff>